<commit_message>
Almost done with SA scripts
</commit_message>
<xml_diff>
--- a/ConsumeSARProj/Manuscript/EVGDescTable.xlsx
+++ b/ConsumeSARProj/Manuscript/EVGDescTable.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FuelsAndEmissions" sheetId="1" r:id="rId1"/>
     <sheet name="EVTAndFB" sheetId="2" r:id="rId2"/>
-    <sheet name="DistributionFits" sheetId="3" r:id="rId3"/>
+    <sheet name="DistributionFitsFlamingFuels" sheetId="3" r:id="rId3"/>
+    <sheet name="DistributionFitsSmolderingFuels" sheetId="4" r:id="rId4"/>
+    <sheet name="SensitivityResults" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>fuels</t>
   </si>
@@ -146,6 +148,18 @@
   </si>
   <si>
     <t>log-normal</t>
+  </si>
+  <si>
+    <t>EVTGroup</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>sensitivityrankSobol</t>
+  </si>
+  <si>
+    <t>SensitivityRankPRCC</t>
   </si>
 </sst>
 </file>
@@ -161,12 +175,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -181,11 +201,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,9 +493,9 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -482,7 +503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -493,7 +514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -517,12 +538,13 @@
       <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -548,7 +570,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>655</v>
       </c>
@@ -562,7 +584,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>682</v>
       </c>
@@ -576,7 +598,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>666</v>
       </c>
@@ -590,7 +612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>683</v>
       </c>
@@ -604,7 +626,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>631</v>
       </c>
@@ -618,7 +640,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>625</v>
       </c>
@@ -639,323 +661,416 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:J1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
+        <v>655</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D3">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E3">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="F3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.11600000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>1.9630000000000001</v>
+      </c>
+      <c r="D4">
+        <v>2.3639999999999999</v>
+      </c>
+      <c r="E4">
+        <v>1.2929999999999999</v>
+      </c>
+      <c r="F4">
+        <v>3.0550000000000002</v>
+      </c>
+      <c r="G4">
+        <v>1.873</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>682</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E8">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="F8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>2.2669999999999999</v>
+      </c>
+      <c r="D9">
+        <v>1.8520000000000001</v>
+      </c>
+      <c r="E9">
+        <v>1.321</v>
+      </c>
+      <c r="F9">
+        <v>2.2320000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>14.619</v>
+      </c>
+      <c r="D10">
+        <v>1.232</v>
+      </c>
+      <c r="E10">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>666</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="4">
+        <v>683</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="4">
+        <v>625</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>27</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>622</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>655</v>
-      </c>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="D3">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E3">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="F3">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="G3">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="J3">
-        <v>0.14799999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>1.9630000000000001</v>
-      </c>
-      <c r="D4">
-        <v>2.3639999999999999</v>
-      </c>
-      <c r="E4">
-        <v>1.2929999999999999</v>
-      </c>
-      <c r="F4">
-        <v>3.0550000000000002</v>
-      </c>
-      <c r="G4">
-        <v>1.873</v>
-      </c>
-      <c r="J4">
-        <v>1.7390000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>682</v>
+        <v>639</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="C8">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D8">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="E8">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="F8">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="J8">
-        <v>4.4999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9">
-        <v>2.2669999999999999</v>
-      </c>
-      <c r="D9">
-        <v>1.8520000000000001</v>
-      </c>
-      <c r="E9">
-        <v>1.321</v>
-      </c>
-      <c r="F9">
-        <v>2.2320000000000002</v>
-      </c>
-      <c r="J9">
-        <v>1.0760000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>24</v>
       </c>
-      <c r="C10">
-        <v>14.619</v>
-      </c>
-      <c r="D10">
-        <v>1.232</v>
-      </c>
-      <c r="E10">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="F10">
-        <v>0.33700000000000002</v>
-      </c>
-      <c r="J10">
-        <v>4.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>631</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>666</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>683</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>631</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>625</v>
-      </c>
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>29</v>
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>